<commit_message>
A model that works but problems with installation costs
Keep this version for old installation cost types.
</commit_message>
<xml_diff>
--- a/projects/CGE_Generator/data/A_IOp.xlsx
+++ b/projects/CGE_Generator/data/A_IOp.xlsx
@@ -12,8 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
-    <sheet name="n" sheetId="1" r:id="rId1"/>
-    <sheet name="i" sheetId="2" r:id="rId2"/>
+    <sheet name="pEqui" sheetId="1" r:id="rId1"/>
+    <sheet name="interestRates" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>a</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>p/p</t>
+  </si>
+  <si>
+    <t>Rrate/t</t>
+  </si>
+  <si>
+    <t>Rrate/Rrate</t>
   </si>
 </sst>
 </file>
@@ -369,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,6 +428,22 @@
         <v>4</v>
       </c>
       <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
         <v>1</v>
       </c>
     </row>
@@ -433,37 +455,144 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U15" sqref="U15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
+      <c r="A2">
+        <v>2016</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0.94788653507940634</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
+      <c r="A3">
+        <v>2017</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>1.0248619914586095</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2018</v>
+      </c>
+      <c r="B4">
+        <v>1.1545674338403451</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2019</v>
+      </c>
+      <c r="B5">
+        <v>1.0375000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2020</v>
+      </c>
+      <c r="B6">
+        <v>1.0409999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2021</v>
+      </c>
+      <c r="B7">
+        <v>1.0450000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2022</v>
+      </c>
+      <c r="B8">
+        <v>1.0480000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2023</v>
+      </c>
+      <c r="B9">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2024</v>
+      </c>
+      <c r="B10">
+        <v>1.0520000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2025</v>
+      </c>
+      <c r="B11">
+        <v>1.054</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2026</v>
+      </c>
+      <c r="B12">
+        <v>1.0560000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2027</v>
+      </c>
+      <c r="B13">
+        <v>1.0580000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2028</v>
+      </c>
+      <c r="B14">
+        <v>1.0589999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2029</v>
+      </c>
+      <c r="B15">
+        <v>1.0609999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2030</v>
+      </c>
+      <c r="B16">
+        <v>1.0619999999999998</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>